<commit_message>
candidate via Keljob/PoleEmploi today 04/07/2018 to dev/integrator
</commit_message>
<xml_diff>
--- a/Candidatures.xlsx
+++ b/Candidatures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="22068" windowHeight="10032"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="22065" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>date</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>plateforme Synergie</t>
+  </si>
+  <si>
+    <t>DEVELOPPEUR-INTEGRATEUR DE LOGICIELS</t>
+  </si>
+  <si>
+    <t>Villeneuve-d'Ascq</t>
+  </si>
+  <si>
+    <t>Pôle Emploi via Keljob</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -431,17 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="6" max="6" width="38.88671875" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -589,6 +602,29 @@
       </c>
       <c r="G6" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>43285</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -603,7 +639,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -615,7 +651,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
plusieurs candidatures au 27/08/2018
</commit_message>
<xml_diff>
--- a/Candidatures.xlsx
+++ b/Candidatures.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
   <si>
     <t>date</t>
   </si>
@@ -172,6 +173,36 @@
   </si>
   <si>
     <t>Développeur Intégrateur Front</t>
+  </si>
+  <si>
+    <t>Développeur Intégrateur de Logiciels</t>
+  </si>
+  <si>
+    <t>pôle emploi</t>
+  </si>
+  <si>
+    <t>Développeur Web</t>
+  </si>
+  <si>
+    <t>Arras</t>
+  </si>
+  <si>
+    <t>Supplay via NordJob</t>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t>Kalyptus</t>
+  </si>
+  <si>
+    <t>Développeur PHP</t>
+  </si>
+  <si>
+    <t>CDi</t>
+  </si>
+  <si>
+    <t>Studio RH</t>
   </si>
 </sst>
 </file>
@@ -523,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -908,6 +939,86 @@
       </c>
       <c r="G16" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>43339</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>43339</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>43339</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>43339</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>